<commit_message>
Fixed python and configs
</commit_message>
<xml_diff>
--- a/models/StarvingStudent_DataModel.xlsx
+++ b/models/StarvingStudent_DataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleshenville/Desktop/TheStarvingStudent/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493096D1-ED3F-5349-B072-49CE12387CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9CAB4A-AE39-E94E-81DE-CF09EFB59A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{468F337A-6BCD-F544-BBC6-95AD1C736E63}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{468F337A-6BCD-F544-BBC6-95AD1C736E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -550,9 +550,6 @@
     <t>https://www.k-cap.com/wp-content/uploads/2018/04/7920.jpg</t>
   </si>
   <si>
-    <t>Ramen Ya @ Sidney Smith Hall 100 St. George St lower level, Toronto, ON M5S 3G3</t>
-  </si>
-  <si>
     <t>https://goo.gl/maps/TnGzuxaJy4Md6YPq7</t>
   </si>
   <si>
@@ -730,9 +727,6 @@
     <t>https://lh5.googleusercontent.com/p/AF1QipPhKKLJ-9rWmK4CPnVFqfC2oQOocSa-RCk38lzY=w408-h272-k-no</t>
   </si>
   <si>
-    <t>Myungrang Hotdog</t>
-  </si>
-  <si>
     <t>https://goo.gl/maps/9LoWr2VgE3b3RZo27</t>
   </si>
   <si>
@@ -751,9 +745,6 @@
     <t>https://wdw.utoronto.ca/sites/default/files/styles/scale_width_811px_/public/assets/images/sidney%20smith%20hall%20cropped.jpg?itok=ViabXdoN</t>
   </si>
   <si>
-    <t>Mike's Cafe @ 81A St. Mary’s St.Brennan Hall, 1st floor Toronto</t>
-  </si>
-  <si>
     <t>https://goo.gl/maps/3SvXoFca4L4vjBaU8</t>
   </si>
   <si>
@@ -830,6 +821,15 @@
   </si>
   <si>
     <t>The Buttery</t>
+  </si>
+  <si>
+    <t>Ramen Ya @ Sidney Smith Hall 100 St, George St lower level, Toronto, ON M5S 3G3</t>
+  </si>
+  <si>
+    <t>Myungrang Hotdog @ 199 College St, Toronto, ON M5T 1P9</t>
+  </si>
+  <si>
+    <t>Mike's Cafe @ 81A St. Marys St, Brennan Hall, 1st floor Toronto</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5CE670-E390-D940-8A79-6269BFF3F570}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1272,10 +1272,10 @@
         <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
@@ -1303,7 +1303,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
@@ -1335,6 +1335,9 @@
         <v>117</v>
       </c>
       <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1359,6 +1362,9 @@
         <v>118</v>
       </c>
       <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1381,6 +1387,9 @@
         <v>119</v>
       </c>
       <c r="H5" s="3"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -1403,6 +1412,9 @@
         <v>120</v>
       </c>
       <c r="H6" s="3"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -1425,6 +1437,9 @@
         <v>122</v>
       </c>
       <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -1447,6 +1462,9 @@
         <v>122</v>
       </c>
       <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1471,6 +1489,9 @@
         <v>128</v>
       </c>
       <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -1495,6 +1516,9 @@
         <v>132</v>
       </c>
       <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1519,6 +1543,9 @@
         <v>135</v>
       </c>
       <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1541,6 +1568,9 @@
         <v>139</v>
       </c>
       <c r="H12" s="3"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -1565,6 +1595,9 @@
         <v>143</v>
       </c>
       <c r="H13" s="3"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1589,6 +1622,9 @@
         <v>147</v>
       </c>
       <c r="H14" s="3"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1613,6 +1649,9 @@
         <v>150</v>
       </c>
       <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1637,8 +1676,11 @@
         <v>154</v>
       </c>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>155</v>
       </c>
@@ -1661,8 +1703,11 @@
         <v>159</v>
       </c>
       <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>160</v>
       </c>
@@ -1685,8 +1730,11 @@
         <v>164</v>
       </c>
       <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>165</v>
       </c>
@@ -1707,10 +1755,13 @@
         <v>169</v>
       </c>
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>170</v>
+        <v>261</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>63</v>
@@ -1719,22 +1770,25 @@
         <v>2.7</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>66</v>
@@ -1743,22 +1797,25 @@
         <v>4</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>66</v>
@@ -1767,22 +1824,25 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>182</v>
-      </c>
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>66</v>
@@ -1791,22 +1851,25 @@
         <v>4.2</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>66</v>
@@ -1815,22 +1878,25 @@
         <v>4.3</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>66</v>
@@ -1839,22 +1905,25 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>63</v>
@@ -1863,7 +1932,7 @@
         <v>2.4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>142</v>
@@ -1872,57 +1941,66 @@
         <v>40</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>63</v>
@@ -1931,22 +2009,25 @@
         <v>4.2</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="H29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>63</v>
@@ -1955,108 +2036,150 @@
         <v>4</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="H30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://maps.google.com/maps?cid=13039585888136325657" xr:uid="{418D742E-AFBB-F04F-AE50-3D1955108C2F}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{8A160917-BB26-F946-8CD0-7F214F15C0FC}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{67D110CF-DCFF-8549-9C05-996393EC2FF5}"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://goo.gl/maps/E9AbvuyDJo87ZaqN8" xr:uid="{13F93404-DACD-2B4C-B29D-7D8F059F2681}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{6B7BBCBD-8865-2E45-B97A-72CCC8E981FB}"/>
-    <hyperlink ref="G3" r:id="rId6" xr:uid="{86808E48-5AD7-4E4C-A02E-D446EE432208}"/>
-    <hyperlink ref="D4" r:id="rId7" xr:uid="{285855B7-2E54-334A-921C-401C1891A88E}"/>
-    <hyperlink ref="E4" r:id="rId8" xr:uid="{67913051-0E0B-8346-9E26-8D4EAA729372}"/>
-    <hyperlink ref="G4" r:id="rId9" xr:uid="{AAE7E8AF-46E1-E942-A8B2-5D84B5717F64}"/>
-    <hyperlink ref="D5" r:id="rId10" xr:uid="{941FDD3A-836B-E44F-9BEA-BE55F2FA79B9}"/>
-    <hyperlink ref="E5" r:id="rId11" xr:uid="{94C542FB-C1F3-7E40-8C62-6B4BDC9C2C7D}"/>
-    <hyperlink ref="G5" r:id="rId12" xr:uid="{C7912E49-EA2D-7F42-83B3-83B26C489A94}"/>
-    <hyperlink ref="D6" r:id="rId13" xr:uid="{B51B3F42-9BC9-AC47-A8C3-B0694C83F5FE}"/>
-    <hyperlink ref="E6" r:id="rId14" xr:uid="{E8EE0A9C-F5B8-0244-BE56-9F9957350DE0}"/>
-    <hyperlink ref="G6" r:id="rId15" xr:uid="{F685A8F3-F03B-9549-A0B1-CE2F0B6032DA}"/>
-    <hyperlink ref="D7" r:id="rId16" xr:uid="{D469F1A3-709A-6445-85CA-2FDD0561CFDF}"/>
-    <hyperlink ref="E7" r:id="rId17" xr:uid="{8D27AA03-A6CC-CF45-8A44-80C40137C18B}"/>
-    <hyperlink ref="G7" r:id="rId18" display="https://www.utoronto.ca/sites/default/files/0J5A0385 copy.jpg" xr:uid="{10922336-7D24-C34D-AE76-DB918389F0EE}"/>
-    <hyperlink ref="D8" r:id="rId19" xr:uid="{40879F5C-8C9D-3F4D-A383-29E5B9D85F23}"/>
-    <hyperlink ref="E8" r:id="rId20" xr:uid="{A957E059-83CD-A141-BEEC-299C11924D02}"/>
-    <hyperlink ref="G8" r:id="rId21" display="https://www.utoronto.ca/sites/default/files/0J5A0385 copy.jpg" xr:uid="{D286E3F6-1C58-914A-BFE7-997D93BBDA47}"/>
-    <hyperlink ref="D9" r:id="rId22" xr:uid="{F588D488-C212-6643-B8E3-D73D1DA67C5A}"/>
-    <hyperlink ref="E9" r:id="rId23" xr:uid="{332F0777-0E59-A740-AD25-7D3D6926E50A}"/>
-    <hyperlink ref="G9" r:id="rId24" xr:uid="{E76CD250-AF1A-C94D-830B-EE6A7A50A81F}"/>
-    <hyperlink ref="D10" r:id="rId25" xr:uid="{D9979AAA-7781-1146-B6FB-52C62912CC1C}"/>
-    <hyperlink ref="E10" r:id="rId26" xr:uid="{33314902-CA8C-6247-855D-EA57E9E97674}"/>
-    <hyperlink ref="G10" r:id="rId27" xr:uid="{33DA5A7F-9970-E440-B43E-A557F7AC08AC}"/>
-    <hyperlink ref="D11" r:id="rId28" xr:uid="{790702BB-5BE2-B445-81DB-E63D4ED36903}"/>
-    <hyperlink ref="E11" r:id="rId29" xr:uid="{FAAE2A97-D237-EF47-8452-61DCBACC4E6B}"/>
-    <hyperlink ref="G11" r:id="rId30" xr:uid="{E01B2D87-A368-8542-AB75-F9223E654FA5}"/>
-    <hyperlink ref="D12" r:id="rId31" xr:uid="{F2E4F682-BF11-6A48-BE54-EDE8A06F485E}"/>
-    <hyperlink ref="E12" r:id="rId32" xr:uid="{FDA75027-1845-2C4C-BED9-B7F2832CD745}"/>
-    <hyperlink ref="G12" r:id="rId33" xr:uid="{357CFD1E-86D7-9847-832B-FA846655A600}"/>
-    <hyperlink ref="D13" r:id="rId34" xr:uid="{AFC44EE9-DAC3-9341-9CF8-1A5899402499}"/>
-    <hyperlink ref="E13" r:id="rId35" xr:uid="{95CF82D2-A1B4-0F46-83EE-8169FB0EDF1F}"/>
-    <hyperlink ref="G13" r:id="rId36" xr:uid="{785A004B-B22B-E64D-8132-0A6AFEC3365A}"/>
-    <hyperlink ref="D14" r:id="rId37" xr:uid="{58DBC4DA-A7AF-CC45-B6FB-06505DD50AD3}"/>
-    <hyperlink ref="E14" r:id="rId38" xr:uid="{D865ED59-B7F9-794F-A3D9-27818D277ADF}"/>
-    <hyperlink ref="G14" r:id="rId39" xr:uid="{D6DAE7EF-4E45-6441-B0C4-55AE14489B22}"/>
-    <hyperlink ref="D15" r:id="rId40" xr:uid="{3D31FCCE-39F9-7B4B-A5BA-3BBAA4F31B3E}"/>
-    <hyperlink ref="E15" r:id="rId41" xr:uid="{75A8A840-05C8-1241-99D3-BF38A48B6A5D}"/>
-    <hyperlink ref="G15" r:id="rId42" xr:uid="{2D2047C5-DFA8-DA47-9124-4B5178B8AF97}"/>
-    <hyperlink ref="D16" r:id="rId43" xr:uid="{2255101E-9D80-6744-ABBA-CA39E1CBB3CD}"/>
-    <hyperlink ref="E16" r:id="rId44" xr:uid="{24173B35-A21F-C342-B2DF-AE647615A917}"/>
-    <hyperlink ref="G16" r:id="rId45" xr:uid="{2BF697B5-6B66-944D-8BBB-5F33E2010E65}"/>
-    <hyperlink ref="D17" r:id="rId46" xr:uid="{9FD0C9E4-726D-0E45-B882-2D83317422AC}"/>
-    <hyperlink ref="E17" r:id="rId47" xr:uid="{7D6AA097-C43A-CD4D-A074-728C3C6AE5AC}"/>
-    <hyperlink ref="G17" r:id="rId48" xr:uid="{98B18FAC-81BE-664E-8556-513388371E82}"/>
-    <hyperlink ref="D18" r:id="rId49" xr:uid="{7AD9B457-D9DE-6D42-97D6-A08470F4879D}"/>
-    <hyperlink ref="E18" r:id="rId50" xr:uid="{CB6840B2-1094-8945-BE41-1CCF5352017A}"/>
-    <hyperlink ref="G18" r:id="rId51" xr:uid="{90281F3E-E40F-B64D-9809-63FD0822E374}"/>
-    <hyperlink ref="D19" r:id="rId52" xr:uid="{45BEB61C-2034-AA41-A32B-7EB285DEEC08}"/>
-    <hyperlink ref="E19" r:id="rId53" xr:uid="{0B80BA1B-6307-4144-B2D2-BC344B2ACBE0}"/>
-    <hyperlink ref="G19" r:id="rId54" xr:uid="{684E3CBD-CC9F-E04B-A67D-C94DEEACCB41}"/>
-    <hyperlink ref="D20" r:id="rId55" xr:uid="{7AB14F6F-AECC-EE43-BD61-596A27956768}"/>
-    <hyperlink ref="E20" r:id="rId56" xr:uid="{5484086D-E045-F24D-A43C-753CE698352A}"/>
-    <hyperlink ref="G20" r:id="rId57" xr:uid="{84E3DE39-C05F-8D49-8DCF-70E7A8C3A65B}"/>
-    <hyperlink ref="D21" r:id="rId58" xr:uid="{D85D0792-E8B9-9F44-A385-9FE4CEA31897}"/>
-    <hyperlink ref="E21" r:id="rId59" xr:uid="{E50161C8-7A9E-ED4A-9D61-4C59B804AA4D}"/>
-    <hyperlink ref="G21" r:id="rId60" xr:uid="{3BFFDCE3-BB67-8847-92E0-D54A30F967C0}"/>
-    <hyperlink ref="D22" r:id="rId61" xr:uid="{6F72A963-1BAD-274D-8BD8-9A163F95F8C7}"/>
-    <hyperlink ref="E22" r:id="rId62" xr:uid="{CA4B33B5-CC44-2D4D-9706-3CD1439F646B}"/>
-    <hyperlink ref="G22" r:id="rId63" xr:uid="{88387223-25E7-4446-8D77-BF9B9CE94BF8}"/>
-    <hyperlink ref="D23" r:id="rId64" xr:uid="{D9D783FB-FDCB-0841-91AB-43B17B5839E3}"/>
-    <hyperlink ref="E23" r:id="rId65" xr:uid="{8703D841-4831-554E-BB48-9FBECEB0313A}"/>
-    <hyperlink ref="G23" r:id="rId66" xr:uid="{D8674D3F-CC5D-A04B-875B-F4AEC7FB4E6B}"/>
-    <hyperlink ref="D24" r:id="rId67" xr:uid="{CB2E12C4-9B57-4946-B583-B6DCC705C142}"/>
-    <hyperlink ref="E24" r:id="rId68" xr:uid="{95C92307-FD10-2442-8457-6B4424738561}"/>
-    <hyperlink ref="G24" r:id="rId69" xr:uid="{C357F96D-5FC6-FB45-AA97-1B50DC05AAFD}"/>
-    <hyperlink ref="D25" r:id="rId70" xr:uid="{62467848-F01E-AD4C-99C3-C8134331C652}"/>
-    <hyperlink ref="E25" r:id="rId71" xr:uid="{39DF007E-D3DA-0A45-AC06-E237E0A85A0E}"/>
-    <hyperlink ref="G25" r:id="rId72" xr:uid="{3A98D40A-DF1E-EC45-B95A-1FCA2987F5CC}"/>
-    <hyperlink ref="D26" r:id="rId73" xr:uid="{8A8F026D-3A75-BE4B-A208-83590C80726F}"/>
-    <hyperlink ref="E26" r:id="rId74" xr:uid="{67817C15-5412-6A46-BC90-D539D86F6ED7}"/>
-    <hyperlink ref="G26" r:id="rId75" display="https://wdw.utoronto.ca/sites/default/files/styles/scale_width_811px_/public/assets/images/sidney smith hall cropped.jpg?itok=ViabXdoN" xr:uid="{69BCD810-4C9A-4F4A-8E20-A6B73A136CEA}"/>
-    <hyperlink ref="D27" r:id="rId76" xr:uid="{357FB9E6-83AA-0146-BE77-2D5C34BCC42B}"/>
-    <hyperlink ref="E27" r:id="rId77" xr:uid="{1B829690-B9D0-D048-92CE-2ADEE54312DB}"/>
-    <hyperlink ref="G27" r:id="rId78" xr:uid="{83B4B9F7-962D-0047-9E12-5985AD24390B}"/>
-    <hyperlink ref="D28" r:id="rId79" xr:uid="{E6E1231C-B2E4-E14E-9D64-EA792837FCEC}"/>
-    <hyperlink ref="E28" r:id="rId80" xr:uid="{3598166C-9917-CA42-8792-396476867838}"/>
-    <hyperlink ref="G28" r:id="rId81" xr:uid="{3E6EBF3D-5444-DD42-9AFB-5AF158F450ED}"/>
-    <hyperlink ref="D29" r:id="rId82" xr:uid="{3BA35FED-C213-0B4A-8A99-9E6FA1B599E2}"/>
-    <hyperlink ref="E29" r:id="rId83" xr:uid="{2ECC8EB3-EBBA-FE41-A361-610DBF4DF434}"/>
-    <hyperlink ref="G29" r:id="rId84" xr:uid="{85E2B051-83AB-F742-9777-A6B4CBC11C89}"/>
-    <hyperlink ref="D30" r:id="rId85" xr:uid="{D238C347-7D15-CF4F-9F5B-485421F37603}"/>
-    <hyperlink ref="E30" r:id="rId86" location="main-content" display="http://www.trinity.utoronto.ca/visit/food-services/buttery.html - main-content" xr:uid="{D0F74786-3EE7-444F-BC13-3709D28E0237}"/>
-    <hyperlink ref="G30" r:id="rId87" xr:uid="{F67BB366-D739-3941-9D12-A24AF388ACD1}"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://maps.google.com/maps?cid=13039585888136325657" xr:uid="{580B2EB7-53DA-D541-9CA9-255E7033CF02}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{178F3F6F-6805-D040-B199-369484B66BA4}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{9F097035-8764-CF4B-BD8D-54A2BFD45FDD}"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://goo.gl/maps/E9AbvuyDJo87ZaqN8" xr:uid="{9D5FE13A-C912-3C40-842A-8B48CC6652B0}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{A11D5EAF-0A0C-E24F-8C6C-2A5C4B83F905}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{FF88152D-61B2-BA40-8F28-E31AFCC87BFB}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{FB1F3241-9B45-EF4E-A230-C7DD98E04572}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{017281CF-D43C-8E49-9FAE-A8AFF929B4CD}"/>
+    <hyperlink ref="G4" r:id="rId9" xr:uid="{E7D2E2FF-A6C3-0A42-A286-4FD8E7412AA5}"/>
+    <hyperlink ref="D5" r:id="rId10" xr:uid="{7731E545-B10B-AF4F-A8F4-EE4AEC6DCC39}"/>
+    <hyperlink ref="E5" r:id="rId11" xr:uid="{B4735F5F-0762-0A48-B65A-C2D19C08A582}"/>
+    <hyperlink ref="G5" r:id="rId12" xr:uid="{2126AE43-611A-C842-8066-E5236FC9EBE0}"/>
+    <hyperlink ref="D6" r:id="rId13" xr:uid="{784C405F-9ED3-FE41-8D18-AE0F3138300E}"/>
+    <hyperlink ref="E6" r:id="rId14" xr:uid="{4F358EDC-5200-E248-8610-80755D7AA6E3}"/>
+    <hyperlink ref="G6" r:id="rId15" xr:uid="{C19BC40E-03D2-5F43-A02C-A9FA58FA1F2A}"/>
+    <hyperlink ref="D7" r:id="rId16" xr:uid="{3880CE28-24D6-1144-87F6-3DD865339A76}"/>
+    <hyperlink ref="E7" r:id="rId17" xr:uid="{6E52007C-D315-6F4F-A860-F28932EE42C4}"/>
+    <hyperlink ref="G7" r:id="rId18" display="https://www.utoronto.ca/sites/default/files/0J5A0385 copy.jpg" xr:uid="{7EB0AA8C-0DFF-2349-AE94-903CCD274DC3}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{89421C35-A9D4-6C48-903B-9D6A51E0F312}"/>
+    <hyperlink ref="E8" r:id="rId20" xr:uid="{2077249C-DFE2-9547-B23D-CCA15D475DFB}"/>
+    <hyperlink ref="G8" r:id="rId21" display="https://www.utoronto.ca/sites/default/files/0J5A0385 copy.jpg" xr:uid="{0756DD2E-A08C-EA41-8958-344C748B8F7E}"/>
+    <hyperlink ref="D9" r:id="rId22" xr:uid="{CAA7F6A4-C24A-4544-9994-DDF1D58A5BA1}"/>
+    <hyperlink ref="E9" r:id="rId23" xr:uid="{276941E0-9385-7749-94E4-019305196B05}"/>
+    <hyperlink ref="G9" r:id="rId24" xr:uid="{B3E4E7D7-6987-1B41-9E35-C6727B7A0ACF}"/>
+    <hyperlink ref="D10" r:id="rId25" xr:uid="{335D011F-9672-0842-B3A2-874F5D260CA1}"/>
+    <hyperlink ref="E10" r:id="rId26" xr:uid="{37D40BC9-5FCE-C14B-BB33-2AD1CBC08319}"/>
+    <hyperlink ref="G10" r:id="rId27" xr:uid="{C86C0DDE-908D-1D4E-A6F7-C7669828BAB4}"/>
+    <hyperlink ref="D11" r:id="rId28" xr:uid="{8CB36906-7AAA-BD4C-ADB6-1861BD7331CD}"/>
+    <hyperlink ref="E11" r:id="rId29" xr:uid="{E6D55843-406A-E541-A0F5-EFFE466D4C04}"/>
+    <hyperlink ref="G11" r:id="rId30" xr:uid="{4809E957-9F1D-AD46-A3F1-2C79ABB625D8}"/>
+    <hyperlink ref="D12" r:id="rId31" xr:uid="{E95C3E0E-B4BD-5649-87B4-C04423BF5335}"/>
+    <hyperlink ref="E12" r:id="rId32" xr:uid="{F419D313-85B6-364D-9A04-0C3E62723350}"/>
+    <hyperlink ref="G12" r:id="rId33" xr:uid="{8A38E8CF-5AC5-9F47-A1E2-1EEDFED2CDB6}"/>
+    <hyperlink ref="D13" r:id="rId34" xr:uid="{17CCBAE1-336B-5D4D-838C-5F09ECFB2774}"/>
+    <hyperlink ref="E13" r:id="rId35" xr:uid="{7F0FB46D-B397-2F4C-A91C-69AEF3DB4D63}"/>
+    <hyperlink ref="G13" r:id="rId36" xr:uid="{3CEBD1ED-7A34-C842-BF46-42E8415AEB18}"/>
+    <hyperlink ref="D14" r:id="rId37" xr:uid="{B68827C1-6159-A044-BDD0-1E32FF3E1E5C}"/>
+    <hyperlink ref="E14" r:id="rId38" xr:uid="{5817CFA2-71DA-5E41-BA47-577A1E1742B9}"/>
+    <hyperlink ref="G14" r:id="rId39" xr:uid="{C87CAEDC-5676-6F47-867C-F440E4A3F459}"/>
+    <hyperlink ref="D15" r:id="rId40" xr:uid="{03C9E702-B5D6-4A40-96D4-0CC50124F155}"/>
+    <hyperlink ref="E15" r:id="rId41" xr:uid="{CE382B8F-874E-F44E-8C61-04EBA56D799A}"/>
+    <hyperlink ref="G15" r:id="rId42" xr:uid="{B02B97E0-C730-CC49-AA97-5F01CDDF3321}"/>
+    <hyperlink ref="D16" r:id="rId43" xr:uid="{CA817E9E-A74A-AD47-88DD-3806E2BF3A72}"/>
+    <hyperlink ref="E16" r:id="rId44" xr:uid="{8BCE960F-746F-744E-BDC3-3B279105260C}"/>
+    <hyperlink ref="G16" r:id="rId45" xr:uid="{7004F74F-A8F3-AE44-83F5-18EFD663361A}"/>
+    <hyperlink ref="D17" r:id="rId46" xr:uid="{0A48A584-7F42-5E46-9B47-7006B78E61B6}"/>
+    <hyperlink ref="E17" r:id="rId47" xr:uid="{6B45A49F-E63B-BC4B-8AE8-990C0649721D}"/>
+    <hyperlink ref="G17" r:id="rId48" xr:uid="{54907D70-E9F6-A948-8CEE-CCC435D94EB6}"/>
+    <hyperlink ref="D18" r:id="rId49" xr:uid="{56739BF3-B0D0-9144-AE37-F422DEB660E5}"/>
+    <hyperlink ref="E18" r:id="rId50" xr:uid="{1CCE595A-9E22-6A4C-9491-750B454ED44B}"/>
+    <hyperlink ref="G18" r:id="rId51" xr:uid="{99D9CA43-2BFB-5341-9D5A-FF6542BEDE0A}"/>
+    <hyperlink ref="D19" r:id="rId52" xr:uid="{DF43ACC8-F1FD-F445-8594-398295A1F0BD}"/>
+    <hyperlink ref="E19" r:id="rId53" xr:uid="{39B80FD0-BAEF-0F4B-9D76-F906B0BA9365}"/>
+    <hyperlink ref="G19" r:id="rId54" xr:uid="{609EC823-5288-454C-BE3D-B8968A568EE8}"/>
+    <hyperlink ref="D20" r:id="rId55" xr:uid="{1F93DB09-005B-5942-AC1C-3AA3E5513CAA}"/>
+    <hyperlink ref="E20" r:id="rId56" xr:uid="{6735807F-2C55-1C4D-A75F-FFF687607015}"/>
+    <hyperlink ref="G20" r:id="rId57" xr:uid="{3AAAC83B-DAA1-1147-A77A-99242579EF62}"/>
+    <hyperlink ref="D21" r:id="rId58" xr:uid="{A8020045-8884-B942-BB81-5BA56F31A19B}"/>
+    <hyperlink ref="E21" r:id="rId59" xr:uid="{C366E458-E92C-C34F-A5C8-D5DA259932CB}"/>
+    <hyperlink ref="G21" r:id="rId60" xr:uid="{57D84770-70E5-D846-9D42-14ECDE1B029C}"/>
+    <hyperlink ref="D22" r:id="rId61" xr:uid="{61B154BA-F4BA-484F-9F6B-90CF2EB36952}"/>
+    <hyperlink ref="E22" r:id="rId62" xr:uid="{56170BA1-5C21-B942-A56A-F882AF548A2F}"/>
+    <hyperlink ref="G22" r:id="rId63" xr:uid="{573C79CE-CA86-2447-8673-4D52CD42AD9B}"/>
+    <hyperlink ref="D23" r:id="rId64" xr:uid="{372C103B-4BFD-A64B-A9A7-1ABC1342D869}"/>
+    <hyperlink ref="E23" r:id="rId65" xr:uid="{0CC4977E-21BD-F342-9973-9752E36C5145}"/>
+    <hyperlink ref="G23" r:id="rId66" xr:uid="{D5C25CAC-17D1-7547-BF64-C29C231792FD}"/>
+    <hyperlink ref="D24" r:id="rId67" xr:uid="{8B03234B-71D6-E44D-9073-2C8162153692}"/>
+    <hyperlink ref="E24" r:id="rId68" xr:uid="{EBCC5D36-39DD-9641-B6D4-41CBC5BF2E13}"/>
+    <hyperlink ref="G24" r:id="rId69" xr:uid="{E952EC84-1A85-2C40-9E4C-1996E61A9A1C}"/>
+    <hyperlink ref="D25" r:id="rId70" xr:uid="{8B542803-D93D-C44C-9A77-E7DEA9D73342}"/>
+    <hyperlink ref="E25" r:id="rId71" xr:uid="{B1A403E2-CDFE-704B-B0B3-4D288F75BCC0}"/>
+    <hyperlink ref="G25" r:id="rId72" xr:uid="{35599BCD-4F04-9744-BC77-B86EA7645686}"/>
+    <hyperlink ref="D26" r:id="rId73" xr:uid="{6D5F6A1D-1856-9249-A9E0-132032046D40}"/>
+    <hyperlink ref="E26" r:id="rId74" xr:uid="{6114C52C-811F-F542-8978-02D16499CC01}"/>
+    <hyperlink ref="G26" r:id="rId75" display="https://wdw.utoronto.ca/sites/default/files/styles/scale_width_811px_/public/assets/images/sidney smith hall cropped.jpg?itok=ViabXdoN" xr:uid="{09EFDF7D-263A-3342-A4B9-AA7C903D50C5}"/>
+    <hyperlink ref="D27" r:id="rId76" xr:uid="{96EAE754-1673-E74A-81ED-77AE3F211A80}"/>
+    <hyperlink ref="E27" r:id="rId77" xr:uid="{925F328E-57D7-A04E-880E-D964B45D18FE}"/>
+    <hyperlink ref="G27" r:id="rId78" xr:uid="{12B976B3-3F2B-6547-B757-7222E56A311F}"/>
+    <hyperlink ref="D28" r:id="rId79" xr:uid="{ED435113-2341-0C44-BCD0-21EB844340E4}"/>
+    <hyperlink ref="E28" r:id="rId80" xr:uid="{EA5B178F-C741-CD43-B219-9E27E350D938}"/>
+    <hyperlink ref="G28" r:id="rId81" xr:uid="{3B50E6AD-96E6-794B-9F36-B0CE1A8C99E5}"/>
+    <hyperlink ref="D29" r:id="rId82" xr:uid="{C037C7AF-8080-3249-94DA-2AE313DA6099}"/>
+    <hyperlink ref="E29" r:id="rId83" xr:uid="{AB9A0AB8-AAA6-BB4F-B08A-548666F7A198}"/>
+    <hyperlink ref="G29" r:id="rId84" xr:uid="{A7ACAA4D-16D4-9947-9E46-133DD9814516}"/>
+    <hyperlink ref="D30" r:id="rId85" xr:uid="{A9BB09ED-2D8F-8741-88F8-C2EA18C97E99}"/>
+    <hyperlink ref="E30" r:id="rId86" location="main-content" display="http://www.trinity.utoronto.ca/visit/food-services/buttery.html - main-content" xr:uid="{CE5DBFAA-4557-7141-A11C-F95103EFA531}"/>
+    <hyperlink ref="G30" r:id="rId87" xr:uid="{F2BF14B8-6CAD-FB4C-8EA4-2B80B00B986A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2169,7 +2292,7 @@
         <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -2197,7 +2320,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2225,7 +2348,7 @@
         <v>52</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2340,26 +2463,26 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -2373,7 +2496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50FB938-05CA-A644-A608-5442697CF5A0}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2390,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>98</v>
@@ -2408,7 +2531,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>99</v>
@@ -2425,7 +2548,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>99</v>
@@ -2442,10 +2565,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2459,10 +2582,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2476,10 +2599,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2493,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2510,7 +2633,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>99</v>
@@ -2527,10 +2650,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2544,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>57</v>
@@ -2561,10 +2684,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2578,7 +2701,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>42</v>
@@ -2595,10 +2718,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2612,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>33</v>
@@ -2629,10 +2752,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2646,10 +2769,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2663,7 +2786,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>110</v>
@@ -2680,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>113</v>
@@ -2691,16 +2814,16 @@
         <v>158</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2708,16 +2831,16 @@
         <v>163</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2725,118 +2848,118 @@
         <v>168</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C24" s="3">
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="C25" s="3">
         <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C27" s="3">
         <v>3</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified configs and fixed cards
</commit_message>
<xml_diff>
--- a/models/StarvingStudent_DataModel.xlsx
+++ b/models/StarvingStudent_DataModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleshenville/Desktop/TheStarvingStudent/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8243099-1894-004E-8609-F57172EF42F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D900796-35D5-704A-AD6A-EE26BCB08006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{468F337A-6BCD-F544-BBC6-95AD1C736E63}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="265">
   <si>
     <t>Restaurant Name</t>
   </si>
@@ -830,6 +830,9 @@
   </si>
   <si>
     <t>StoreImage</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1250,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,7 +1280,9 @@
       <c r="H1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -2189,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839D75C0-0B2E-4E4C-87AF-285A2FCFECD3}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2496,8 +2501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50FB938-05CA-A644-A608-5442697CF5A0}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>